<commit_message>
Skills Higher Quals fixes.
</commit_message>
<xml_diff>
--- a/dashboard_loader/skills_higher_qual_uploader/skills_higher_qual.xlsx
+++ b/dashboard_loader/skills_higher_qual_uploader/skills_higher_qual.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -53,10 +53,10 @@
     <t xml:space="preserve">Aust</t>
   </si>
   <si>
-    <t xml:space="preserve">Diploma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Advanced Diploma</t>
+    <t xml:space="preserve">Dip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adv Dip</t>
   </si>
   <si>
     <t xml:space="preserve">Status</t>
@@ -364,11 +364,14 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N28" activeCellId="0" sqref="N28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.9234693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1131,8 +1134,8 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="E25:E26 A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>